<commit_message>
Update results wiht the abs error
</commit_message>
<xml_diff>
--- a/Result_different_algorithm_2.xlsx
+++ b/Result_different_algorithm_2.xlsx
@@ -96,7 +96,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -175,16 +175,66 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
       <right style="thick">
         <color indexed="64"/>
       </right>
       <top/>
       <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -193,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -223,13 +273,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -237,6 +284,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -644,7 +712,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -658,35 +726,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="G1" s="15" t="s">
+      <c r="B1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
     </row>
     <row r="2" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="11"/>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="10"/>
+      <c r="B2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="18" t="s">
         <v>15</v>
       </c>
       <c r="G2" s="3" t="s">
@@ -780,13 +850,13 @@
         <v>2</v>
       </c>
       <c r="C6" s="4">
-        <v>11</v>
+        <v>11.9</v>
       </c>
       <c r="D6" s="9">
         <v>2.2999999999999998</v>
       </c>
       <c r="E6" s="4">
-        <v>11</v>
+        <v>11.4</v>
       </c>
       <c r="F6" s="9">
         <v>2.2000000000000002</v>
@@ -808,22 +878,22 @@
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14" t="s">
+      <c r="B10" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
     </row>
     <row r="11" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="13"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="3" t="s">
         <v>4</v>
       </c>
@@ -900,9 +970,9 @@
   <mergeCells count="5">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B1:D1"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="E10:G10"/>
+    <mergeCell ref="B1:F1"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:C6">
     <cfRule type="colorScale" priority="5">

</xml_diff>